<commit_message>
added averages to samples.xlsx
</commit_message>
<xml_diff>
--- a/samples/samples.xlsx
+++ b/samples/samples.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Saad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Saad\Documents\CompSci\NYU\bayesian_ml\project\gpt-2\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F652E50-8052-4AA9-B068-BBA8645A4BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4CF578-05BA-4C33-BA10-CE1CA2B69119}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{85DD4D70-A0CB-4D54-B5AD-9502E8E88775}"/>
   </bookViews>
@@ -121,8 +121,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -138,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -146,18 +154,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="double">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -4599,7 +4624,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D0CF82B3-F65F-47D9-B911-916D6034525A}" name="Name"/>
     <tableColumn id="2" xr3:uid="{C79C9548-A00A-4881-ACC8-ABDDFB8801BA}" name="Size"/>
-    <tableColumn id="3" xr3:uid="{559B4E7A-1F50-4C09-BEF5-6D3573C11F86}" name="Percent" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{559B4E7A-1F50-4C09-BEF5-6D3573C11F86}" name="Percent" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4639,11 +4664,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0D208B0D-24FC-491F-9F93-8053081984BF}" name="Table9" displayName="Table9" ref="A29:C34" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0D208B0D-24FC-491F-9F93-8053081984BF}" name="Table9" displayName="Table9" ref="A29:C35" totalsRowCount="1">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E9CB99E0-6B28-4F1B-8B7B-AF979F646DB1}" name="Name"/>
     <tableColumn id="2" xr3:uid="{A9E3E8B8-E143-404E-A221-27E66A4B4158}" name="Size"/>
-    <tableColumn id="3" xr3:uid="{A716AF04-B0C1-4EEC-AA8B-9BF7C06DFAB2}" name="Percent" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{A716AF04-B0C1-4EEC-AA8B-9BF7C06DFAB2}" name="Percent" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+      <totalsRowFormula>AVERAGE(C4,C11,C18,C25,C32)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4947,10 +4974,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E072F783-5C15-4223-BABD-A90FB2D01A23}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5300,6 +5327,24 @@
       </c>
       <c r="C34" s="1">
         <v>0.98540000000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C35" s="1">
+        <f>AVERAGE(C4,C11,C18,C25,C32)</f>
+        <v>0.75503999999999993</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C36" s="2">
+        <f>AVERAGE(C5,C12,C19,C26,C33)</f>
+        <v>0.71245999999999987</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C37">
+        <f>C36/Table9[[#Totals],[Percent]]*100</f>
+        <v>94.360563678745493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>